<commit_message>
current updates to sheets thingy
</commit_message>
<xml_diff>
--- a/OSL-2019.xlsx
+++ b/OSL-2019.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="203">
   <si>
     <t>artist</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>sure why not</t>
+  </si>
+  <si>
     <t>Lil Wayne</t>
   </si>
   <si>
@@ -73,12 +76,18 @@
     <t>3:35-4:25 PM</t>
   </si>
   <si>
+    <t>I mean it literally will be sweater weather</t>
+  </si>
+  <si>
     <t>P-Lo</t>
   </si>
   <si>
     <t>2:20-3:05 PM</t>
   </si>
   <si>
+    <t>locally sourced hyphy</t>
+  </si>
+  <si>
     <t>Half Alive</t>
   </si>
   <si>
@@ -88,7 +97,7 @@
     <t>Riff Magazine</t>
   </si>
   <si>
-    <t>Good live Long Beach rock?</t>
+    <t>Good live Long Beach rock? Early but fun early day music</t>
   </si>
   <si>
     <t>Taylor Bennett</t>
@@ -97,7 +106,7 @@
     <t>noon-12:40 PM</t>
   </si>
   <si>
-    <t>Jazzy rap</t>
+    <t>Jazzy rap ... have literally never gotten there this early</t>
   </si>
   <si>
     <t>Flying Lotus 3D</t>
@@ -109,24 +118,39 @@
     <t>8:40-9:40 PM</t>
   </si>
   <si>
+    <t>For the visuals alone ... instrumental trip-hop if that makes sense?</t>
+  </si>
+  <si>
     <t>San Holo</t>
   </si>
   <si>
     <t>7:20-8:10 PM</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>not feeling it at all ... so much treble</t>
+  </si>
+  <si>
     <t>Yaeji</t>
   </si>
   <si>
     <t>6-6:50 PM</t>
   </si>
   <si>
+    <t>Maybe a bit mellow, but per wikipedia: Her style blends elements of house music and hip hop with mellow, quiet vocals sung in both English and Korean.</t>
+  </si>
+  <si>
     <t>Masego</t>
   </si>
   <si>
     <t>4:40-5:30 PM</t>
   </si>
   <si>
+    <t>TrapHouseJazz, seems mellow and potentially solid live</t>
+  </si>
+  <si>
     <t>Still Woozy</t>
   </si>
   <si>
@@ -145,12 +169,18 @@
     <t>2:05-2:50 PM</t>
   </si>
   <si>
+    <t>like ambient R&amp;B pretty cool</t>
+  </si>
+  <si>
     <t>The Seshen</t>
   </si>
   <si>
     <t>12:50-1:35 PM</t>
   </si>
   <si>
+    <t>local "live electronic" so probs good if unlikely to get there</t>
+  </si>
+  <si>
     <t>The Lumineers</t>
   </si>
   <si>
@@ -163,19 +193,25 @@
     <t>SF Chronicle</t>
   </si>
   <si>
+    <t>Unless Nina likes them? But Flylo probs &gt;&gt;&gt;</t>
+  </si>
+  <si>
     <t>Counting Crows</t>
   </si>
   <si>
     <t>6:50-7:50 PM</t>
   </si>
   <si>
+    <t>There are like two songs</t>
+  </si>
+  <si>
     <t>Lauren Daigle</t>
   </si>
   <si>
     <t>5:15-6:05 PM</t>
   </si>
   <si>
-    <t>Christian…</t>
+    <t>Christian solo vocalist</t>
   </si>
   <si>
     <t>Aurora</t>
@@ -184,18 +220,27 @@
     <t>3:40-4:30 PM</t>
   </si>
   <si>
+    <t>Norwegian Electropop ... might be great but early listens have me skeptical</t>
+  </si>
+  <si>
     <t>The California Honeydrops</t>
   </si>
   <si>
     <t>2:05-2:55 PM</t>
   </si>
   <si>
+    <t>Oakland "Roots" and R&amp;B band but they're all white? Probs fun live tho</t>
+  </si>
+  <si>
     <t>Grateful Shred</t>
   </si>
   <si>
     <t>12:40-1:20 PM</t>
   </si>
   <si>
+    <t>Grateful dead cover band kill me now</t>
+  </si>
+  <si>
     <t>Luttrell</t>
   </si>
   <si>
@@ -205,7 +250,7 @@
     <t>7:50-8:35 PM</t>
   </si>
   <si>
-    <t>Melodic techno</t>
+    <t>Melodic techno ... like 75% lighter than techno bunker ... techno atrium or some shit</t>
   </si>
   <si>
     <t>Brasstracks</t>
@@ -214,7 +259,7 @@
     <t>6:05-6:45 PM</t>
   </si>
   <si>
-    <t>Brassy EDM (Chance the Rappers last album)</t>
+    <t>Brassy EDM (Chance the Rappers last album) probably good</t>
   </si>
   <si>
     <t>The Marias</t>
@@ -223,21 +268,33 @@
     <t>4:30-5:10 PM</t>
   </si>
   <si>
+    <t>https://remezcla.com/features/music/the-marias-interview/</t>
+  </si>
+  <si>
     <t>Miya Folick</t>
   </si>
   <si>
     <t>2:55-3:35 PM</t>
   </si>
   <si>
+    <t>described as folk rock so no</t>
+  </si>
+  <si>
     <t>Boyfriend</t>
   </si>
   <si>
     <t>1:20-2 PM</t>
   </si>
   <si>
+    <t>for the description on the app alone</t>
+  </si>
+  <si>
     <t>Rainbow Girls</t>
   </si>
   <si>
+    <t>from SB, sounds like acoustic soul?</t>
+  </si>
+  <si>
     <t>Childish Gambino</t>
   </si>
   <si>
@@ -485,9 +542,6 @@
   </si>
   <si>
     <t>2-2:45 PM</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>"Genre-blurred hip hop" … super not feeling it</t>
@@ -575,7 +629,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dddd, mmm. d"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -585,6 +639,10 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -601,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -613,6 +671,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,11 +762,13 @@
         <v>14</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -714,19 +777,19 @@
         <v>43686.0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -735,15 +798,19 @@
         <v>43686.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -752,15 +819,19 @@
         <v>43686.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -769,19 +840,21 @@
         <v>43686.0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -790,366 +863,432 @@
         <v>43686.0</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2">
         <v>43686.0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2">
         <v>43686.0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2">
         <v>43686.0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2">
         <v>43686.0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2">
         <v>43686.0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2">
         <v>43686.0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2">
         <v>43686.0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C16" s="2">
         <v>43686.0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2">
         <v>43686.0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2">
         <v>43686.0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F18" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2">
         <v>43686.0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="G19" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C20" s="2">
         <v>43686.0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C21" s="2">
         <v>43686.0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2">
         <v>43686.0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2">
         <v>43686.0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F23" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C24" s="2">
         <v>43686.0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C25" s="2">
         <v>43686.0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C26" s="2">
         <v>43686.0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C27" s="2">
         <v>43686.0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>8</v>
@@ -1164,15 +1303,15 @@
         <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
@@ -1187,12 +1326,13 @@
         <v>10</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G29" s="1"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
@@ -1201,7 +1341,7 @@
         <v>43687.0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1209,7 +1349,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>8</v>
@@ -1218,18 +1358,19 @@
         <v>43687.0</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>8</v>
@@ -1238,7 +1379,7 @@
         <v>43687.0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1246,7 +1387,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>8</v>
@@ -1255,7 +1396,7 @@
         <v>43687.0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1263,7 +1404,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>8</v>
@@ -1272,7 +1413,7 @@
         <v>43687.0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1280,36 +1421,37 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C35" s="2">
         <v>43687.0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G35" s="1"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C36" s="2">
         <v>43687.0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1317,16 +1459,16 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C37" s="2">
         <v>43687.0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1334,16 +1476,16 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C38" s="2">
         <v>43687.0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1351,16 +1493,16 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C39" s="2">
         <v>43687.0</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1368,16 +1510,16 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2">
         <v>43687.0</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1385,16 +1527,16 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2">
+        <v>43687.0</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C41" s="2">
-        <v>43687.0</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1402,16 +1544,16 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C42" s="2">
         <v>43687.0</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -1419,34 +1561,35 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C43" s="2">
         <v>43687.0</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G43" s="1"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C44" s="2">
         <v>43687.0</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -1454,58 +1597,58 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2">
         <v>43687.0</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="1" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C46" s="2">
         <v>43687.0</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C47" s="2">
         <v>43687.0</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -1513,16 +1656,16 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C48" s="2">
         <v>43687.0</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -1530,16 +1673,16 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C49" s="2">
         <v>43687.0</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -1547,16 +1690,16 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C50" s="2">
         <v>43687.0</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -1564,16 +1707,16 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C51" s="2">
         <v>43687.0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -1581,16 +1724,16 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C52" s="2">
         <v>43687.0</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -1598,16 +1741,16 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C53" s="2">
         <v>43687.0</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -1615,7 +1758,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>8</v>
@@ -1624,18 +1767,19 @@
         <v>43688.0</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G54" s="1"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>8</v>
@@ -1644,7 +1788,7 @@
         <v>43688.0</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>10</v>
@@ -1654,7 +1798,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>8</v>
@@ -1663,21 +1807,21 @@
         <v>43688.0</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>8</v>
@@ -1686,7 +1830,7 @@
         <v>43688.0</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -1694,7 +1838,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>8</v>
@@ -1703,7 +1847,7 @@
         <v>43688.0</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -1711,7 +1855,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>8</v>
@@ -1720,73 +1864,74 @@
         <v>43688.0</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C60" s="2">
         <v>43688.0</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C61" s="2">
         <v>43688.0</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G61" s="1"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C62" s="2">
         <v>43688.0</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -1794,16 +1939,16 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C63" s="2">
         <v>43688.0</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -1811,16 +1956,16 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C64" s="2">
         <v>43688.0</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -1828,16 +1973,16 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C65" s="2">
         <v>43688.0</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -1845,16 +1990,16 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C66" s="2">
         <v>43688.0</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -1862,16 +2007,16 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C67" s="2">
         <v>43688.0</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -1879,16 +2024,16 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C68" s="2">
         <v>43688.0</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -1896,16 +2041,16 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C69" s="2">
         <v>43688.0</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -1913,62 +2058,62 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C70" s="2">
         <v>43688.0</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C71" s="2">
         <v>43688.0</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C72" s="2">
         <v>43688.0</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -1976,39 +2121,39 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C73" s="2">
         <v>43688.0</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C74" s="2">
         <v>43688.0</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -2016,16 +2161,16 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C75" s="2">
         <v>43688.0</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -2033,16 +2178,16 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C76" s="2">
         <v>43688.0</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -2050,16 +2195,16 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C77" s="2">
         <v>43688.0</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -2067,16 +2212,16 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C78" s="2">
         <v>43688.0</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
@@ -2084,99 +2229,92 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C79" s="2">
         <v>43687.0</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="1" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C80" s="2">
         <v>43687.0</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F80" s="3"/>
       <c r="G80" s="1" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C81" s="2">
         <v>43687.0</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="1" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C82" s="2">
         <v>43687.0</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="1" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F61:G61"/>
-  </mergeCells>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G24"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated figures and figure code with text for acts and output that works well on phone screen
</commit_message>
<xml_diff>
--- a/OSL-2019.xlsx
+++ b/OSL-2019.xlsx
@@ -11,11 +11,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="263">
   <si>
     <t>artist</t>
   </si>
   <si>
+    <t>artist_simp</t>
+  </si>
+  <si>
     <t>stage</t>
   </si>
   <si>
@@ -34,9 +37,15 @@
     <t>comments</t>
   </si>
   <si>
+    <t>nina</t>
+  </si>
+  <si>
     <t>Twenty One Pilots</t>
   </si>
   <si>
+    <t>21 Pilots</t>
+  </si>
+  <si>
     <t>Lands End Stage</t>
   </si>
   <si>
@@ -73,6 +82,9 @@
     <t>The Neighborhood</t>
   </si>
   <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
     <t>3:35-4:25 PM</t>
   </si>
   <si>
@@ -88,6 +100,9 @@
     <t>locally sourced hyphy</t>
   </si>
   <si>
+    <t xml:space="preserve">NINA LIKES IT </t>
+  </si>
+  <si>
     <t>Half Alive</t>
   </si>
   <si>
@@ -103,6 +118,9 @@
     <t>Taylor Bennett</t>
   </si>
   <si>
+    <t>T-Bennett</t>
+  </si>
+  <si>
     <t>noon-12:40 PM</t>
   </si>
   <si>
@@ -112,6 +130,9 @@
     <t>Flying Lotus 3D</t>
   </si>
   <si>
+    <t>Flying Lotus</t>
+  </si>
+  <si>
     <t>Sutro Stage</t>
   </si>
   <si>
@@ -166,6 +187,9 @@
     <t>Cautious Clay</t>
   </si>
   <si>
+    <t>CautiousClay</t>
+  </si>
+  <si>
     <t>2:05-2:50 PM</t>
   </si>
   <si>
@@ -175,6 +199,9 @@
     <t>The Seshen</t>
   </si>
   <si>
+    <t>Seshen</t>
+  </si>
+  <si>
     <t>12:50-1:35 PM</t>
   </si>
   <si>
@@ -184,6 +211,9 @@
     <t>The Lumineers</t>
   </si>
   <si>
+    <t>Lumineers</t>
+  </si>
+  <si>
     <t>Twin Peaks Stage</t>
   </si>
   <si>
@@ -226,6 +256,9 @@
     <t>The California Honeydrops</t>
   </si>
   <si>
+    <t>CA Honeydrops</t>
+  </si>
+  <si>
     <t>2:05-2:55 PM</t>
   </si>
   <si>
@@ -352,6 +385,9 @@
     <t>Better Oblivion Community Center</t>
   </si>
   <si>
+    <t>Better Oblivion</t>
+  </si>
+  <si>
     <t>6:15-7:05 PM</t>
   </si>
   <si>
@@ -361,6 +397,9 @@
     <t>Phosphorescent</t>
   </si>
   <si>
+    <t>Phosphor.</t>
+  </si>
+  <si>
     <t>4:55-5:45 PM</t>
   </si>
   <si>
@@ -370,6 +409,9 @@
     <t>Edie Brickell &amp; New Bohemians</t>
   </si>
   <si>
+    <t>Edie Brickell</t>
+  </si>
+  <si>
     <t>3:40-4:25 PM</t>
   </si>
   <si>
@@ -388,6 +430,9 @@
     <t>Haley Heynderickx</t>
   </si>
   <si>
+    <t>Heynderickx</t>
+  </si>
+  <si>
     <t>1:10-1:55 PM</t>
   </si>
   <si>
@@ -514,12 +559,15 @@
     <t>4:10-5:10 PM</t>
   </si>
   <si>
-    <t>Country but really good</t>
+    <t>"Country but really good" ~ music press. "Overplayed sad girl with guitar" ~ Nina Bingham</t>
   </si>
   <si>
     <t>Judah &amp; the Lion</t>
   </si>
   <si>
+    <t>JudahLion</t>
+  </si>
+  <si>
     <t>2:50-3:40 PM</t>
   </si>
   <si>
@@ -535,6 +583,9 @@
     <t>oldschool soul</t>
   </si>
   <si>
+    <t xml:space="preserve">REALLY CHILL IF WERE TIRED </t>
+  </si>
+  <si>
     <t>PJ Morton</t>
   </si>
   <si>
@@ -550,6 +601,9 @@
     <t>Anderson .Paak and the Free Nationals</t>
   </si>
   <si>
+    <t>Anderson .Paak</t>
+  </si>
+  <si>
     <t>7:30-8:30 PM</t>
   </si>
   <si>
@@ -574,33 +628,54 @@
     <t>dark dance?</t>
   </si>
   <si>
+    <t>NINA SAYS TURMSTASSE-y</t>
+  </si>
+  <si>
     <t>DJ Koze</t>
   </si>
   <si>
+    <t>enthusiastic techno would be one way to say it?</t>
+  </si>
+  <si>
     <t>Dean Lewis</t>
   </si>
   <si>
+    <t>IF SAD A BOY WITH GUITARS HAD KEYBOARDS INSTEAD</t>
+  </si>
+  <si>
     <t>Cherry Glazerr</t>
   </si>
   <si>
+    <t>Synthpop</t>
+  </si>
+  <si>
     <t>Weyes Blood</t>
   </si>
   <si>
     <t>noon-12:45 PM</t>
   </si>
   <si>
+    <t>Melancholy and psychedelic</t>
+  </si>
+  <si>
     <t>Kygo</t>
   </si>
   <si>
     <t>8:20-9:35 PM</t>
   </si>
   <si>
+    <t>Paul Simon better</t>
+  </si>
+  <si>
     <t>Bebe Rexha</t>
   </si>
   <si>
     <t>6:40-7:35 PM</t>
   </si>
   <si>
+    <t>Toro y Moi better</t>
+  </si>
+  <si>
     <t>Sheck Wes</t>
   </si>
   <si>
@@ -616,9 +691,15 @@
     <t>Trap rap great live … pretty intense lyrically … really solid beats</t>
   </si>
   <si>
+    <t xml:space="preserve">RLY RLY INTENSE </t>
+  </si>
+  <si>
     <t>Nahko &amp; Medicine for the People</t>
   </si>
   <si>
+    <t>Nahko</t>
+  </si>
+  <si>
     <t>2-2:45 PM</t>
   </si>
   <si>
@@ -649,21 +730,33 @@
     <t>4:20-5 PM</t>
   </si>
   <si>
+    <t>ambient</t>
+  </si>
+  <si>
     <t>Jupiter &amp; Okwess</t>
   </si>
   <si>
+    <t>Jupiter&amp;Okwess</t>
+  </si>
+  <si>
     <t>2:45-3:25 PM</t>
   </si>
   <si>
     <t>Alex Lahey</t>
   </si>
   <si>
+    <t>Sounds like a fun thing to check out</t>
+  </si>
+  <si>
     <t>Sandys</t>
   </si>
   <si>
     <t>Back-to-Back with Molly Baz</t>
   </si>
   <si>
+    <t>Molly</t>
+  </si>
+  <si>
     <t>GastroMagic</t>
   </si>
   <si>
@@ -676,6 +769,9 @@
     <t>Big Wild (MCed by AR)</t>
   </si>
   <si>
+    <t>(AR)</t>
+  </si>
+  <si>
     <t>3:10-3:40 PM</t>
   </si>
   <si>
@@ -685,6 +781,9 @@
     <t>Slurpers (CupcakKe and Andy)</t>
   </si>
   <si>
+    <t>Andy</t>
+  </si>
+  <si>
     <t>4:25-4:55 PM</t>
   </si>
   <si>
@@ -692,6 +791,9 @@
   </si>
   <si>
     <t>Test Kitchen Live (errebody)</t>
+  </si>
+  <si>
+    <t>TKL</t>
   </si>
   <si>
     <t>5:45-6:15 PM</t>
@@ -707,7 +809,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dddd, mmm. d"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -718,6 +820,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
@@ -737,12 +840,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -750,7 +856,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -776,7 +882,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="33.14"/>
-    <col customWidth="1" min="3" max="3" width="15.57"/>
+    <col customWidth="1" min="4" max="4" width="15.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -801,1698 +907,1997 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="D11" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2">
+        <v>53</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2">
+        <v>58</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="2">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="2">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="2">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>66</v>
+        <v>32</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="D19" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="2">
+        <v>81</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="2">
+        <v>84</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="2">
+        <v>87</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>79</v>
+        <v>32</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="2">
+        <v>91</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>82</v>
+        <v>32</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="2">
+        <v>94</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4" t="s">
-        <v>85</v>
+        <v>95</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="2">
+        <v>97</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="2">
+        <v>100</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="2">
+        <v>103</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="3">
         <v>43686.0</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="1" t="s">
-        <v>93</v>
+        <v>36</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="2">
+        <v>105</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="2">
+        <v>108</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>98</v>
+        <v>69</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="2">
+        <v>110</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="1" t="s">
-        <v>100</v>
+        <v>20</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="2">
+        <v>112</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>102</v>
+        <v>69</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="2">
+        <v>114</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="1" t="s">
-        <v>104</v>
+        <v>27</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="2">
+        <v>116</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="1" t="s">
-        <v>106</v>
+        <v>31</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="2">
+        <v>118</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="1" t="s">
-        <v>108</v>
+        <v>36</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="2">
+        <v>120</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>111</v>
+        <v>69</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="2">
+        <v>124</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="2">
+        <v>128</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="1" t="s">
-        <v>117</v>
+        <v>129</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="4"/>
+      <c r="H37" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="2">
+        <v>132</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="2">
+        <v>135</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="E39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="1" t="s">
-        <v>123</v>
+        <v>136</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="2">
+        <v>139</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="E40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="1" t="s">
-        <v>126</v>
+        <v>140</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="2">
+        <v>142</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="1" t="s">
-        <v>128</v>
+        <v>36</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" s="2">
+        <v>144</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="3"/>
-      <c r="G42" s="1" t="s">
-        <v>130</v>
+        <v>68</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" s="2">
+        <v>146</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E43" s="1" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>100</v>
+        <v>69</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="2">
+        <v>147</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="1" t="s">
-        <v>134</v>
+        <v>148</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="2">
+        <v>150</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>138</v>
+        <v>152</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="2">
+        <v>154</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="E46" s="1" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>141</v>
+        <v>32</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="2">
+        <v>157</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="3"/>
-      <c r="G47" s="1" t="s">
-        <v>144</v>
+        <v>158</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="2">
+        <v>160</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="3"/>
-      <c r="G48" s="1" t="s">
-        <v>146</v>
+        <v>89</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="2">
+        <v>162</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="E49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="1" t="s">
-        <v>149</v>
+        <v>163</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C50" s="2">
+        <v>165</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="E50" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F50" s="3"/>
-      <c r="G50" s="1" t="s">
-        <v>152</v>
+        <v>166</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C51" s="2">
+        <v>168</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="E51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" s="3"/>
-      <c r="G51" s="1" t="s">
-        <v>155</v>
+        <v>169</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" s="2">
+        <v>171</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="3"/>
-      <c r="G52" s="1" t="s">
-        <v>158</v>
+        <v>172</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C53" s="2">
+        <v>174</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D53" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="E53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="2">
+        <v>175</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G54" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H54" s="1"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="2">
+        <v>177</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="1" t="s">
-        <v>164</v>
+        <v>178</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="4"/>
+      <c r="H55" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="2">
+        <v>180</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="E56" s="1" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>167</v>
+        <v>106</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="2">
+        <v>184</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>170</v>
+        <v>185</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="2">
+        <v>187</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="E58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="3"/>
-      <c r="G58" s="1" t="s">
-        <v>173</v>
+        <v>188</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="2">
+        <v>191</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>177</v>
+        <v>193</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C60" s="2">
+        <v>196</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="E60" s="1" t="s">
-        <v>10</v>
+        <v>197</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>180</v>
+        <v>152</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C61" s="2">
+        <v>199</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>14</v>
+        <v>200</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>183</v>
+        <v>69</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C62" s="2">
+        <v>202</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F62" s="3"/>
-      <c r="G62" s="1" t="s">
-        <v>186</v>
+        <v>203</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="2">
+        <v>206</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
+      <c r="E63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="4"/>
+      <c r="H63" s="1" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C64" s="2">
+        <v>208</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
+      <c r="E64" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G64" s="4"/>
+      <c r="H64" s="1" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C65" s="2">
+        <v>210</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
+      <c r="E65" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="4"/>
+      <c r="H65" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C66" s="2">
+        <v>212</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
+      <c r="E66" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G66" s="4"/>
+      <c r="H66" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C67" s="2">
+        <v>215</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
+      <c r="E67" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="4"/>
+      <c r="H67" s="1" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" s="2">
+        <v>218</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
+      <c r="E68" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="1" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C69" s="2">
+        <v>221</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D69" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
+      <c r="E69" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" s="2">
+        <v>223</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="E70" s="1" t="s">
-        <v>10</v>
+        <v>224</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>200</v>
+        <v>32</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C71" s="2">
+        <v>228</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D71" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="E71" s="1" t="s">
-        <v>38</v>
+        <v>229</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>203</v>
+        <v>32</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C72" s="2">
+        <v>231</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
+      <c r="E72" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C73" s="2">
+        <v>232</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D73" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="E73" s="1" t="s">
-        <v>10</v>
+        <v>233</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>207</v>
+        <v>32</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C74" s="2">
+        <v>235</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D74" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
+      <c r="E74" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F74" s="1"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="1"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" s="2">
+        <v>237</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
+      <c r="E75" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" s="4"/>
+      <c r="H75" s="1" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C76" s="2">
+        <v>241</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
+      <c r="E76" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" s="2">
+        <v>243</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D77" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
+      <c r="E77" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G77" s="4"/>
+      <c r="H77" s="1" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" s="2">
+        <v>245</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78" s="3">
         <v>43688.0</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
+      <c r="E78" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C79" s="2">
+        <v>247</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D79" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="E79" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F79" s="3"/>
-      <c r="G79" s="1" t="s">
-        <v>219</v>
+        <v>249</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G79" s="4"/>
+      <c r="H79" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C80" s="2">
+        <v>252</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D80" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="E80" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="3"/>
-      <c r="G80" s="1" t="s">
-        <v>222</v>
+        <v>253</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G80" s="4"/>
+      <c r="H80" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C81" s="2">
+        <v>256</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D81" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="E81" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="3"/>
-      <c r="G81" s="1" t="s">
-        <v>225</v>
+        <v>257</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G81" s="4"/>
+      <c r="H81" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>226</v>
+        <v>259</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C82" s="2">
+        <v>260</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D82" s="3">
         <v>43687.0</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="E82" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="3"/>
-      <c r="G82" s="1" t="s">
-        <v>228</v>
+        <v>261</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" s="4"/>
+      <c r="H82" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G24"/>
+    <hyperlink r:id="rId1" ref="H24"/>
   </hyperlinks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>